<commit_message>
Analisis de la red
</commit_message>
<xml_diff>
--- a/CSV/Interactions.xlsx
+++ b/CSV/Interactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azaid\OneDrive - UNIVERSIDAD NACIONAL AUTÓNOMA DE MÉXICO\lcg\lab yalbi\Macrophage_Boolean_Network\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DCA749-3F52-4CEC-8EAE-7E71D1AB17C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD42F18E-639A-4B9E-BF51-B334CA0C3CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F06A6ED-7FB8-4556-B07E-08C82FD4F1CE}"/>
   </bookViews>
@@ -761,16 +761,16 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="25.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -807,7 +807,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -824,7 +824,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -844,7 +844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -864,7 +864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -881,7 +881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -895,7 +895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -912,7 +912,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -932,7 +932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -949,7 +949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -964,7 +964,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -984,7 +984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="3"/>
     </row>
   </sheetData>

</xml_diff>